<commit_message>
update beranda_lowongan_mahasiswa & template jurusan
</commit_message>
<xml_diff>
--- a/template-mapping/insert-template-jurusan.xlsx
+++ b/template-mapping/insert-template-jurusan.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\AgitCRM\CRM\template-mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training-Material\Project\Project CRM\Code\CRM\template-mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
   <si>
     <t>idJurusan</t>
   </si>
@@ -50,16 +50,505 @@
     <t>Teknik Informatika</t>
   </si>
   <si>
-    <t>Desain Grafis</t>
-  </si>
-  <si>
     <t>Kedokteran Gigi</t>
   </si>
   <si>
     <t>Teknik Sipil</t>
   </si>
   <si>
-    <t>Hukum</t>
+    <t>Agribisnis</t>
+  </si>
+  <si>
+    <t>Agronomi</t>
+  </si>
+  <si>
+    <t>Agroteknologi</t>
+  </si>
+  <si>
+    <t>Akuntansi</t>
+  </si>
+  <si>
+    <t>Antropologi Sosial</t>
+  </si>
+  <si>
+    <t>Jur06</t>
+  </si>
+  <si>
+    <t>Arkeologi</t>
+  </si>
+  <si>
+    <t>Jur07</t>
+  </si>
+  <si>
+    <t>Arsitektur</t>
+  </si>
+  <si>
+    <t>Jur08</t>
+  </si>
+  <si>
+    <t>Biokimia</t>
+  </si>
+  <si>
+    <t>Jur09</t>
+  </si>
+  <si>
+    <t>Biologi</t>
+  </si>
+  <si>
+    <t>Jur10</t>
+  </si>
+  <si>
+    <t>Bioteknologi/Teknobiologi</t>
+  </si>
+  <si>
+    <t>Jur11</t>
+  </si>
+  <si>
+    <t>Budidaya Perairan</t>
+  </si>
+  <si>
+    <t>Jur12</t>
+  </si>
+  <si>
+    <t>Jur13</t>
+  </si>
+  <si>
+    <t>Farmasi</t>
+  </si>
+  <si>
+    <t>Jur14</t>
+  </si>
+  <si>
+    <t>Geofisika</t>
+  </si>
+  <si>
+    <t>Jur15</t>
+  </si>
+  <si>
+    <t>Ilmu Administrasi Negara</t>
+  </si>
+  <si>
+    <t>Jur16</t>
+  </si>
+  <si>
+    <t>Ilmu Administrasi Niaga</t>
+  </si>
+  <si>
+    <t>Jur17</t>
+  </si>
+  <si>
+    <t>Ilmu EKonomi</t>
+  </si>
+  <si>
+    <t>Jur18</t>
+  </si>
+  <si>
+    <t>Ilmu Filsafat</t>
+  </si>
+  <si>
+    <t>Jur19</t>
+  </si>
+  <si>
+    <t>Ilmu Gizi</t>
+  </si>
+  <si>
+    <t>Jur20</t>
+  </si>
+  <si>
+    <t>Ilmu Hubungan Internasional</t>
+  </si>
+  <si>
+    <t>Jur21</t>
+  </si>
+  <si>
+    <t>Ilmu Kelautan</t>
+  </si>
+  <si>
+    <t>Jur22</t>
+  </si>
+  <si>
+    <t>Ilmu Keperawatan</t>
+  </si>
+  <si>
+    <t>Jur23</t>
+  </si>
+  <si>
+    <t>Ilmu Kesejahteraan Sosial</t>
+  </si>
+  <si>
+    <t>Jur24</t>
+  </si>
+  <si>
+    <t>Ilmu Komputer</t>
+  </si>
+  <si>
+    <t>Jur25</t>
+  </si>
+  <si>
+    <t>Ilmu Komunikasi</t>
+  </si>
+  <si>
+    <t>Jur26</t>
+  </si>
+  <si>
+    <t>Ilmu Perpustakaan</t>
+  </si>
+  <si>
+    <t>Jur27</t>
+  </si>
+  <si>
+    <t>Ilmu Politik</t>
+  </si>
+  <si>
+    <t>Jur28</t>
+  </si>
+  <si>
+    <t>Ilmu Sejarah</t>
+  </si>
+  <si>
+    <t>Jur29</t>
+  </si>
+  <si>
+    <t>Ilmu Tanah</t>
+  </si>
+  <si>
+    <t>Jur30</t>
+  </si>
+  <si>
+    <t>Kebidanan</t>
+  </si>
+  <si>
+    <t>Jur31</t>
+  </si>
+  <si>
+    <t>Kedokteran</t>
+  </si>
+  <si>
+    <t>Jur32</t>
+  </si>
+  <si>
+    <t>Jur33</t>
+  </si>
+  <si>
+    <t>Kedokteran Hewan</t>
+  </si>
+  <si>
+    <t>Jur34</t>
+  </si>
+  <si>
+    <t>Kehutanan</t>
+  </si>
+  <si>
+    <t>Jur35</t>
+  </si>
+  <si>
+    <t>Kesehatan Masyarakat</t>
+  </si>
+  <si>
+    <t>Jur36</t>
+  </si>
+  <si>
+    <t>Kimia</t>
+  </si>
+  <si>
+    <t>Jur37</t>
+  </si>
+  <si>
+    <t>Manajemen</t>
+  </si>
+  <si>
+    <t>Jur38</t>
+  </si>
+  <si>
+    <t>Manajemen Sumberdaya Perairan</t>
+  </si>
+  <si>
+    <t>Jur39</t>
+  </si>
+  <si>
+    <t>Meteorologi</t>
+  </si>
+  <si>
+    <t>Jur40</t>
+  </si>
+  <si>
+    <t>Pendidikan Biologi</t>
+  </si>
+  <si>
+    <t>Jur41</t>
+  </si>
+  <si>
+    <t>Pendidikan Fisika</t>
+  </si>
+  <si>
+    <t>Jur42</t>
+  </si>
+  <si>
+    <t>Pendidikan Kimia</t>
+  </si>
+  <si>
+    <t>Jur43</t>
+  </si>
+  <si>
+    <t>Pendidikan Matematika</t>
+  </si>
+  <si>
+    <t>Jur44</t>
+  </si>
+  <si>
+    <t>Perencanaan Wilayah dan Tata Kota</t>
+  </si>
+  <si>
+    <t>Jur45</t>
+  </si>
+  <si>
+    <t>Peternakan</t>
+  </si>
+  <si>
+    <t>Jur46</t>
+  </si>
+  <si>
+    <t>Sastra Arab</t>
+  </si>
+  <si>
+    <t>Jur47</t>
+  </si>
+  <si>
+    <t>Sastra Belanda</t>
+  </si>
+  <si>
+    <t>Jur48</t>
+  </si>
+  <si>
+    <t>Sastra Cina</t>
+  </si>
+  <si>
+    <t>Jur49</t>
+  </si>
+  <si>
+    <t>Sastra Indonesia</t>
+  </si>
+  <si>
+    <t>Jur50</t>
+  </si>
+  <si>
+    <t>Sastra Inggris</t>
+  </si>
+  <si>
+    <t>Jur51</t>
+  </si>
+  <si>
+    <t>Sastra Jawa</t>
+  </si>
+  <si>
+    <t>Jur52</t>
+  </si>
+  <si>
+    <t>Sastra Jepang</t>
+  </si>
+  <si>
+    <t>Jur53</t>
+  </si>
+  <si>
+    <t>Sastra Jerman</t>
+  </si>
+  <si>
+    <t>Jur54</t>
+  </si>
+  <si>
+    <t>Sastra Korea</t>
+  </si>
+  <si>
+    <t>Jur55</t>
+  </si>
+  <si>
+    <t>Sastra Perancis</t>
+  </si>
+  <si>
+    <t>Jur56</t>
+  </si>
+  <si>
+    <t>Sastra Rusia</t>
+  </si>
+  <si>
+    <t>Jur57</t>
+  </si>
+  <si>
+    <t>Sistem Informasi</t>
+  </si>
+  <si>
+    <t>Jur58</t>
+  </si>
+  <si>
+    <t>Sosiologi</t>
+  </si>
+  <si>
+    <t>Jur59</t>
+  </si>
+  <si>
+    <t>Statistika</t>
+  </si>
+  <si>
+    <t>Jur60</t>
+  </si>
+  <si>
+    <t>Teknik Bangunan</t>
+  </si>
+  <si>
+    <t>Jur61</t>
+  </si>
+  <si>
+    <t>Teknik Elektro</t>
+  </si>
+  <si>
+    <t>Jur62</t>
+  </si>
+  <si>
+    <t>Teknik Fisika</t>
+  </si>
+  <si>
+    <t>Jur63</t>
+  </si>
+  <si>
+    <t>Teknik geodesi</t>
+  </si>
+  <si>
+    <t>Jur64</t>
+  </si>
+  <si>
+    <t>Teknik Geologi</t>
+  </si>
+  <si>
+    <t>Jur65</t>
+  </si>
+  <si>
+    <t>Teknik Industri</t>
+  </si>
+  <si>
+    <t>Jur66</t>
+  </si>
+  <si>
+    <t>Teknik industri</t>
+  </si>
+  <si>
+    <t>Jur67</t>
+  </si>
+  <si>
+    <t>Jur68</t>
+  </si>
+  <si>
+    <t>Teknik Kimia</t>
+  </si>
+  <si>
+    <t>Jur69</t>
+  </si>
+  <si>
+    <t>Teknik kimia</t>
+  </si>
+  <si>
+    <t>Jur70</t>
+  </si>
+  <si>
+    <t>Teknik Komputer</t>
+  </si>
+  <si>
+    <t>Jur71</t>
+  </si>
+  <si>
+    <t>Teknik Lingkungan</t>
+  </si>
+  <si>
+    <t>Jur72</t>
+  </si>
+  <si>
+    <t>Teknik Mesin</t>
+  </si>
+  <si>
+    <t>Jur73</t>
+  </si>
+  <si>
+    <t>Teknik mesin</t>
+  </si>
+  <si>
+    <t>Jur74</t>
+  </si>
+  <si>
+    <t>Teknik Metalurgi dan Material</t>
+  </si>
+  <si>
+    <t>Jur75</t>
+  </si>
+  <si>
+    <t>Teknik nuklir</t>
+  </si>
+  <si>
+    <t>Jur76</t>
+  </si>
+  <si>
+    <t>Teknik Penerbangan</t>
+  </si>
+  <si>
+    <t>Jur77</t>
+  </si>
+  <si>
+    <t>Teknik Perkapalan</t>
+  </si>
+  <si>
+    <t>Jur78</t>
+  </si>
+  <si>
+    <t>Teknik Perminyakan</t>
+  </si>
+  <si>
+    <t>Jur79</t>
+  </si>
+  <si>
+    <t>Teknik Pertambangan</t>
+  </si>
+  <si>
+    <t>Jur80</t>
+  </si>
+  <si>
+    <t>Teknik pertanian</t>
+  </si>
+  <si>
+    <t>Jur81</t>
+  </si>
+  <si>
+    <t>Teknik Planologi</t>
+  </si>
+  <si>
+    <t>Jur82</t>
+  </si>
+  <si>
+    <t>Jur83</t>
+  </si>
+  <si>
+    <t>Teknik sipil</t>
+  </si>
+  <si>
+    <t>Jur84</t>
+  </si>
+  <si>
+    <t>Teknologi industri pertanian</t>
+  </si>
+  <si>
+    <t>Jur85</t>
+  </si>
+  <si>
+    <t>Teknologi informasi</t>
+  </si>
+  <si>
+    <t>Jur86</t>
+  </si>
+  <si>
+    <t>Teknologi Pangan</t>
+  </si>
+  <si>
+    <t>Jur87</t>
+  </si>
+  <si>
+    <t>Teknologi pangan dan hasil pertanian</t>
   </si>
 </sst>
 </file>
@@ -378,22 +867,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,44 +890,700 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>